<commit_message>
FINAL PAPA GOL DE COLOMBIA
</commit_message>
<xml_diff>
--- a/Docs/ISIS1225 - Tablas de Datos Lab 7.xlsx
+++ b/Docs/ISIS1225 - Tablas de Datos Lab 7.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28723"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Linds\Desktop\Liv-stuff\MAESTRIA\SEGUNDO SEMESTRE\ASISTENCIA\lab 7 JP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FE89C1-6036-4B20-A2C9-FA3316217E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC507FA8-F618-4A1D-AAAC-71842D28D641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="767" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,8 +116,25 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,18 +143,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor theme="0" tint="-0.14999847407452621"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -165,11 +176,73 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -183,16 +256,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -204,89 +271,41 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <b val="0"/>
@@ -336,32 +355,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -455,7 +448,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -624,8 +617,20 @@
             <c:numRef>
               <c:f>'Datos Lab7'!$B$3:$B$6</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6250.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1250.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>892.875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>694.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -633,8 +638,20 @@
             <c:numRef>
               <c:f>'Datos Lab7'!$C$3:$C$6</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3237.44</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>870.06</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>627.61</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>621.82000000000005</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -731,8 +748,20 @@
             <c:numRef>
               <c:f>'Datos Lab7'!$B$11:$B$14</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>546.79999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>273.39999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>182.32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>136.71</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -740,8 +769,20 @@
             <c:numRef>
               <c:f>'Datos Lab7'!$C$11:$C$14</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>280.14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>212.45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>182.99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>185.24</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -839,7 +880,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -964,7 +1005,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1079,7 +1120,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1297,8 +1338,20 @@
             <c:numRef>
               <c:f>'Datos Lab7'!$B$3:$B$6</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6250.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1250.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>892.875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>694.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1443,8 +1496,20 @@
             <c:numRef>
               <c:f>'Datos Lab7'!$B$11:$B$14</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>546.79999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>273.39999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>182.32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>136.71</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1645,7 +1710,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2908,33 +2973,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A2:C6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A2:C6" xr:uid="{B245DDE7-54F2-4A7A-AC17-5CA17DD7B03F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A10:C14" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A10:C14" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Factor de Carga (PROBING)"/>
-    <tableColumn id="5" xr3:uid="{F280BCD9-1105-4F25-860B-4E27D28E75B2}" name="Consumo de Datos [kB]" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Tiempo de Ejecución Real @LP [ms]" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Factor de Carga (CHAINING)" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{89028F05-533D-401C-8D1A-1C8737D88894}" name="Consumo de Datos [kB]"/>
+    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Tiempo de Ejecución Real @SC [ms]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A10:C14" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A10:C14" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A2:C6" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A2:C6" xr:uid="{B245DDE7-54F2-4A7A-AC17-5CA17DD7B03F}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Factor de Carga (CHAINING)" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{89028F05-533D-401C-8D1A-1C8737D88894}" name="Consumo de Datos [kB]" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Tiempo de Ejecución Real @SC [ms]" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Factor de Carga (PROBING)"/>
+    <tableColumn id="5" xr3:uid="{F280BCD9-1105-4F25-860B-4E27D28E75B2}" name="Consumo de Datos [kB]"/>
+    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Tiempo de Ejecución Real @LP [ms]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2972,7 +3037,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3078,7 +3143,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3220,7 +3285,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3231,24 +3296,24 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:C14"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="27.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:3" ht="18.75">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
-    <row r="2" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" ht="30.75">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -3259,81 +3324,113 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="8">
+    <row r="3" spans="1:3" ht="15">
+      <c r="A3" s="6">
         <v>0.1</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="7"/>
+      <c r="B3" s="19">
+        <v>6250.6</v>
+      </c>
+      <c r="C3" s="16">
+        <v>3237.44</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="9">
+    <row r="4" spans="1:3" ht="15">
+      <c r="A4" s="7">
         <v>0.5</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="7"/>
+      <c r="B4" s="12">
+        <v>1250.3</v>
+      </c>
+      <c r="C4" s="13">
+        <v>870.06</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="8">
+    <row r="5" spans="1:3" ht="15">
+      <c r="A5" s="6">
         <v>0.7</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="7"/>
+      <c r="B5" s="10">
+        <v>892.875</v>
+      </c>
+      <c r="C5" s="11">
+        <v>627.61</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="10">
+    <row r="6" spans="1:3" ht="15">
+      <c r="A6" s="8">
         <v>0.9</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="7"/>
+      <c r="B6" s="14">
+        <v>694.5</v>
+      </c>
+      <c r="C6" s="15">
+        <v>621.82000000000005</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.45">
-      <c r="A9" s="11" t="s">
+    <row r="9" spans="1:3" ht="18">
+      <c r="A9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
     </row>
-    <row r="10" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" ht="28.5">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" ht="15">
       <c r="A11" s="2">
         <v>2</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="5"/>
+      <c r="B11" s="17">
+        <v>546.79999999999995</v>
+      </c>
+      <c r="C11" s="16">
+        <v>280.14</v>
+      </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" ht="15">
       <c r="A12" s="2">
         <v>4</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="12">
+        <v>273.39999999999998</v>
+      </c>
+      <c r="C12" s="13">
+        <v>212.45</v>
+      </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" ht="15">
       <c r="A13" s="2">
         <v>6</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="B13" s="10">
+        <v>182.32</v>
+      </c>
+      <c r="C13" s="18">
+        <v>182.99</v>
+      </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" ht="15">
       <c r="A14" s="2">
         <v>8</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="B14" s="14">
+        <v>136.71</v>
+      </c>
+      <c r="C14" s="15">
+        <v>185.24</v>
+      </c>
     </row>
-    <row r="23" ht="14.65" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="23" ht="14.65" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
@@ -3348,12 +3445,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="164883f8-7691-4ecf-b54a-664c0d0edefe">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3606,50 +3705,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="164883f8-7691-4ecf-b54a-664c0d0edefe">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E10B9E65-6C88-4633-81F7-F02338B2B10B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
-    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E10B9E65-6C88-4633-81F7-F02338B2B10B}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
-    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}"/>
 </file>
</xml_diff>